<commit_message>
updated data input sheet
</commit_message>
<xml_diff>
--- a/app/src/main/resources/AutomationExercise_DataInputSheet.xlsx
+++ b/app/src/main/resources/AutomationExercise_DataInputSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Sr.</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Mobile Number</t>
   </si>
   <si>
-    <t>JoeDoe</t>
+    <t>JonyL</t>
   </si>
   <si>
     <t>Mr</t>
@@ -91,10 +91,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Doe</t>
+    <t>Jony</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>Example Corp</t>
@@ -106,7 +106,7 @@
     <t>Apt 4B</t>
   </si>
   <si>
-    <t>USA</t>
+    <t>United States</t>
   </si>
   <si>
     <t>California</t>
@@ -115,7 +115,7 @@
     <t>Los Angeles</t>
   </si>
   <si>
-    <t>HarrySmith</t>
+    <t>ShyamP</t>
   </si>
   <si>
     <t>Mrs</t>
@@ -127,10 +127,10 @@
     <t>December</t>
   </si>
   <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Smith</t>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
   <si>
     <t>Test Inc</t>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Suite 5</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
   <si>
     <t>New York</t>
@@ -838,7 +841,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="11">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>24</v>
@@ -862,13 +865,13 @@
         <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R3" s="11">
         <v>10001</v>

</xml_diff>